<commit_message>
adding space on top of y axis and removing outlier in take home plot
</commit_message>
<xml_diff>
--- a/FishLandings/household groups/statistics summary.xlsx
+++ b/FishLandings/household groups/statistics summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Kenya_SamakiSalama\FishLandings\household groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914DE7DA-0842-488E-AB26-71D9BAB2F972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CAE58B-10C0-4E57-A868-B076702D68E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31125" yWindow="3390" windowWidth="21600" windowHeight="11235" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="118">
   <si>
     <t>Effect</t>
   </si>
@@ -217,9 +217,6 @@
     <t>0.45 ± 0.11 (4)</t>
   </si>
   <si>
-    <t>0.79 ± 0.29 (18)</t>
-  </si>
-  <si>
     <t>1.44 ± 0.13 (29)</t>
   </si>
   <si>
@@ -383,6 +380,9 @@
   </si>
   <si>
     <t>71.97 ± 6.06 (71)</t>
+  </si>
+  <si>
+    <t>0.51 ± 0.08 (17)</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -731,9 +731,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E06F813-7338-485B-A007-E93757D85C7B}">
   <dimension ref="B3:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,7 +1063,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -1071,7 +1078,7 @@
         <v>52</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>7</v>
@@ -1086,7 +1093,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="47" t="s">
         <v>8</v>
@@ -1103,7 +1110,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -1118,7 +1125,7 @@
         <v>52</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>7</v>
@@ -1133,7 +1140,7 @@
         <v>55</v>
       </c>
       <c r="D9" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="47" t="s">
         <v>8</v>
@@ -1150,7 +1157,7 @@
         <v>53</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -1165,7 +1172,7 @@
         <v>52</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>7</v>
@@ -1180,7 +1187,7 @@
         <v>55</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="47" t="s">
         <v>8</v>
@@ -1197,7 +1204,7 @@
         <v>53</v>
       </c>
       <c r="D13" s="58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>6</v>
@@ -1212,7 +1219,7 @@
         <v>52</v>
       </c>
       <c r="D14" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>7</v>
@@ -1227,7 +1234,7 @@
         <v>55</v>
       </c>
       <c r="D15" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="47" t="s">
         <v>8</v>
@@ -1244,7 +1251,7 @@
         <v>53</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
@@ -1259,7 +1266,7 @@
         <v>52</v>
       </c>
       <c r="D17" s="58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>7</v>
@@ -1274,7 +1281,7 @@
         <v>55</v>
       </c>
       <c r="D18" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" s="47" t="s">
         <v>8</v>
@@ -1291,7 +1298,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>6</v>
@@ -1306,7 +1313,7 @@
         <v>52</v>
       </c>
       <c r="D20" s="58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>7</v>
@@ -1321,7 +1328,7 @@
         <v>55</v>
       </c>
       <c r="D21" s="60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21" s="47" t="s">
         <v>8</v>
@@ -1338,7 +1345,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
@@ -1353,7 +1360,7 @@
         <v>52</v>
       </c>
       <c r="D23" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
@@ -1368,7 +1375,7 @@
         <v>55</v>
       </c>
       <c r="D24" s="60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" s="47" t="s">
         <v>8</v>
@@ -1385,7 +1392,7 @@
         <v>53</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" s="48" t="s">
         <v>6</v>
@@ -1400,7 +1407,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>7</v>
@@ -1415,7 +1422,7 @@
         <v>55</v>
       </c>
       <c r="D27" s="60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
@@ -1432,7 +1439,7 @@
         <v>53</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>6</v>
@@ -1447,7 +1454,7 @@
         <v>52</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>7</v>
@@ -1462,7 +1469,7 @@
         <v>55</v>
       </c>
       <c r="D30" s="60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E30" s="47" t="s">
         <v>8</v>
@@ -1479,7 +1486,7 @@
         <v>53</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>6</v>
@@ -1494,7 +1501,7 @@
         <v>52</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E32" s="53" t="s">
         <v>7</v>
@@ -1509,7 +1516,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33" s="47" t="s">
         <v>8</v>
@@ -1526,7 +1533,7 @@
         <v>53</v>
       </c>
       <c r="D34" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>6</v>
@@ -1541,7 +1548,7 @@
         <v>52</v>
       </c>
       <c r="D35" s="58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>7</v>
@@ -1556,7 +1563,7 @@
         <v>55</v>
       </c>
       <c r="D36" s="60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E36" s="47" t="s">
         <v>8</v>
@@ -1573,7 +1580,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>6</v>
@@ -1588,7 +1595,7 @@
         <v>52</v>
       </c>
       <c r="D38" s="58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>7</v>
@@ -1603,7 +1610,7 @@
         <v>55</v>
       </c>
       <c r="D39" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E39" s="47" t="s">
         <v>8</v>
@@ -1620,7 +1627,7 @@
         <v>53</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>6</v>
@@ -1635,7 +1642,7 @@
         <v>52</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>7</v>
@@ -1650,7 +1657,7 @@
         <v>55</v>
       </c>
       <c r="D42" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>8</v>
@@ -1667,7 +1674,7 @@
         <v>53</v>
       </c>
       <c r="D43" s="58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>6</v>
@@ -1682,7 +1689,7 @@
         <v>52</v>
       </c>
       <c r="D44" s="58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>7</v>
@@ -1697,7 +1704,7 @@
         <v>55</v>
       </c>
       <c r="D45" s="60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>8</v>
@@ -1767,7 +1774,7 @@
         <v>6</v>
       </c>
       <c r="F49" s="31">
-        <v>0.77264200000000005</v>
+        <v>0.97677599999999998</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1776,13 +1783,13 @@
         <v>52</v>
       </c>
       <c r="D50" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="E50" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E50" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="31">
-        <v>0.11310199999999999</v>
+      <c r="F50" s="34">
+        <v>7.3119999999999999E-3</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1791,13 +1798,13 @@
         <v>55</v>
       </c>
       <c r="D51" s="60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E51" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F51" s="35">
-        <v>5.6349999999999997E-2</v>
+      <c r="F51" s="67" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1808,7 +1815,7 @@
         <v>53</v>
       </c>
       <c r="D52" s="58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E52" s="53" t="s">
         <v>6</v>
@@ -1823,7 +1830,7 @@
         <v>52</v>
       </c>
       <c r="D53" s="58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>7</v>
@@ -1838,7 +1845,7 @@
         <v>55</v>
       </c>
       <c r="D54" s="60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E54" s="47" t="s">
         <v>8</v>
@@ -1855,7 +1862,7 @@
         <v>53</v>
       </c>
       <c r="D55" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>6</v>
@@ -1870,7 +1877,7 @@
         <v>52</v>
       </c>
       <c r="D56" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>7</v>
@@ -1885,7 +1892,7 @@
         <v>55</v>
       </c>
       <c r="D57" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>8</v>
@@ -1902,7 +1909,7 @@
         <v>53</v>
       </c>
       <c r="D58" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>6</v>
@@ -1917,7 +1924,7 @@
         <v>52</v>
       </c>
       <c r="D59" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E59" s="53" t="s">
         <v>7</v>
@@ -1932,7 +1939,7 @@
         <v>55</v>
       </c>
       <c r="D60" s="60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E60" s="47" t="s">
         <v>8</v>
@@ -1949,7 +1956,7 @@
         <v>53</v>
       </c>
       <c r="D61" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E61" s="53" t="s">
         <v>6</v>
@@ -1964,7 +1971,7 @@
         <v>52</v>
       </c>
       <c r="D62" s="58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>7</v>
@@ -1979,7 +1986,7 @@
         <v>55</v>
       </c>
       <c r="D63" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E63" s="47" t="s">
         <v>8</v>
@@ -1998,7 +2005,7 @@
   <dimension ref="B1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2126,7 +2133,7 @@
         <v>53</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>6</v>
@@ -2149,7 +2156,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>7</v>
@@ -2172,7 +2179,7 @@
         <v>55</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>8</v>
@@ -2292,7 +2299,7 @@
         <v>53</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>6</v>
@@ -2315,7 +2322,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>7</v>
@@ -2338,7 +2345,7 @@
         <v>55</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>8</v>
@@ -2522,7 +2529,7 @@
         <v>53</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>6</v>
@@ -2545,7 +2552,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>7</v>
@@ -2568,7 +2575,7 @@
         <v>55</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>8</v>
@@ -2688,7 +2695,7 @@
         <v>53</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>6</v>
@@ -2711,7 +2718,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>7</v>
@@ -2734,7 +2741,7 @@
         <v>55</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>8</v>
@@ -2854,7 +2861,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>6</v>
@@ -2877,7 +2884,7 @@
         <v>52</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>7</v>
@@ -2900,7 +2907,7 @@
         <v>55</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>8</v>
@@ -3020,7 +3027,7 @@
         <v>53</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>6</v>
@@ -3043,7 +3050,7 @@
         <v>52</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>7</v>
@@ -3066,7 +3073,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" s="27" t="s">
         <v>8</v>
@@ -3186,7 +3193,7 @@
         <v>53</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>6</v>
@@ -3209,7 +3216,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>7</v>
@@ -3232,7 +3239,7 @@
         <v>55</v>
       </c>
       <c r="C46" s="60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46" s="27" t="s">
         <v>8</v>
@@ -3352,7 +3359,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D53" s="39" t="s">
         <v>6</v>
@@ -3375,7 +3382,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D54" s="23" t="s">
         <v>7</v>
@@ -3398,7 +3405,7 @@
         <v>55</v>
       </c>
       <c r="C55" s="60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D55" s="33" t="s">
         <v>8</v>
@@ -3518,7 +3525,7 @@
         <v>53</v>
       </c>
       <c r="C62" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D62" s="39" t="s">
         <v>6</v>
@@ -3541,7 +3548,7 @@
         <v>52</v>
       </c>
       <c r="C63" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D63" s="23" t="s">
         <v>7</v>
@@ -3564,7 +3571,7 @@
         <v>55</v>
       </c>
       <c r="C64" s="60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D64" s="27" t="s">
         <v>8</v>
@@ -3725,7 +3732,7 @@
         <v>53</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>6</v>
@@ -3748,7 +3755,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>7</v>
@@ -3771,7 +3778,7 @@
         <v>55</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>8</v>
@@ -3891,7 +3898,7 @@
         <v>53</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>6</v>
@@ -3914,7 +3921,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>7</v>
@@ -3937,7 +3944,7 @@
         <v>55</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>8</v>
@@ -4057,7 +4064,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>6</v>
@@ -4080,7 +4087,7 @@
         <v>52</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>7</v>
@@ -4103,7 +4110,7 @@
         <v>55</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>8</v>
@@ -4223,7 +4230,7 @@
         <v>53</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>6</v>
@@ -4246,7 +4253,7 @@
         <v>52</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>7</v>
@@ -4269,7 +4276,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37" s="33" t="s">
         <v>8</v>
@@ -4389,7 +4396,7 @@
         <v>53</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>6</v>
@@ -4412,7 +4419,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>7</v>
@@ -4435,7 +4442,7 @@
         <v>55</v>
       </c>
       <c r="C46" s="60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" s="33" t="s">
         <v>8</v>
@@ -4579,8 +4586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FFC064-2F91-4093-9CA2-53F2C36B19E0}">
   <dimension ref="B1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4802,17 +4809,17 @@
       <c r="D13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="64">
         <v>0.80072299999999996</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="64">
         <v>1</v>
       </c>
-      <c r="G13" s="22">
-        <v>0.96716299999999999</v>
+      <c r="G13" s="64">
+        <v>2.3380879999999999</v>
       </c>
       <c r="H13" s="31">
-        <v>0.33032</v>
+        <v>0.13294700000000001</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -4823,17 +4830,17 @@
       <c r="D14" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="30">
-        <v>6.6748919999999998</v>
-      </c>
-      <c r="F14" s="30">
+      <c r="E14" s="68">
+        <v>10.704165</v>
+      </c>
+      <c r="F14" s="68">
         <v>2</v>
       </c>
-      <c r="G14" s="30">
-        <v>4.0311729999999999</v>
-      </c>
-      <c r="H14" s="34">
-        <v>2.4081000000000002E-2</v>
+      <c r="G14" s="68">
+        <v>15.627917999999999</v>
+      </c>
+      <c r="H14" s="69" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -4842,13 +4849,13 @@
       <c r="D15" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="22">
-        <v>39.739646999999998</v>
-      </c>
-      <c r="F15" s="22">
-        <v>48</v>
-      </c>
-      <c r="G15" s="22"/>
+      <c r="E15" s="64">
+        <v>16.096057999999999</v>
+      </c>
+      <c r="F15" s="64">
+        <v>47</v>
+      </c>
+      <c r="G15" s="64"/>
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4880,17 +4887,17 @@
       <c r="D17" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="25">
-        <v>0.34512700000000002</v>
-      </c>
-      <c r="F17" s="25">
-        <v>-0.87128399999999995</v>
-      </c>
-      <c r="G17" s="25">
-        <v>1.5615380000000001</v>
+      <c r="E17" s="65">
+        <v>6.7158999999999996E-2</v>
+      </c>
+      <c r="F17" s="65">
+        <v>-0.71989300000000001</v>
+      </c>
+      <c r="G17" s="65">
+        <v>0.85421000000000002</v>
       </c>
       <c r="H17" s="31">
-        <v>0.77264200000000005</v>
+        <v>0.97677599999999998</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -4898,22 +4905,22 @@
         <v>52</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="66">
         <v>0.99118700000000004</v>
       </c>
-      <c r="F18" s="25">
-        <v>-0.18253</v>
-      </c>
-      <c r="G18" s="25">
-        <v>2.1649029999999998</v>
-      </c>
-      <c r="H18" s="31">
-        <v>0.11310199999999999</v>
+      <c r="F18" s="66">
+        <v>0.235788</v>
+      </c>
+      <c r="G18" s="66">
+        <v>1.7465850000000001</v>
+      </c>
+      <c r="H18" s="34">
+        <v>7.3119999999999999E-3</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
@@ -4921,22 +4928,22 @@
         <v>55</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="65">
-        <v>0.64605900000000005</v>
-      </c>
-      <c r="F19" s="65">
-        <v>-1.4252000000000001E-2</v>
-      </c>
-      <c r="G19" s="65">
-        <v>1.3063709999999999</v>
-      </c>
-      <c r="H19" s="66">
-        <v>5.6349999999999997E-2</v>
+      <c r="E19" s="28">
+        <v>0.92402799999999996</v>
+      </c>
+      <c r="F19" s="28">
+        <v>0.49141099999999999</v>
+      </c>
+      <c r="G19" s="28">
+        <v>1.3566450000000001</v>
+      </c>
+      <c r="H19" s="67" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5041,7 +5048,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" s="29" t="s">
         <v>6</v>
@@ -5064,7 +5071,7 @@
         <v>52</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>7</v>
@@ -5087,7 +5094,7 @@
         <v>55</v>
       </c>
       <c r="C28" s="60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>8</v>
@@ -5207,7 +5214,7 @@
         <v>53</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D35" s="23" t="s">
         <v>6</v>
@@ -5230,7 +5237,7 @@
         <v>52</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>7</v>
@@ -5253,7 +5260,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D37" s="33" t="s">
         <v>8</v>
@@ -5373,7 +5380,7 @@
         <v>53</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>6</v>
@@ -5396,7 +5403,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D45" s="29" t="s">
         <v>7</v>
@@ -5419,7 +5426,7 @@
         <v>55</v>
       </c>
       <c r="C46" s="60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D46" s="27" t="s">
         <v>8</v>
@@ -5539,7 +5546,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D53" s="29" t="s">
         <v>6</v>
@@ -5562,7 +5569,7 @@
         <v>52</v>
       </c>
       <c r="C54" s="58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D54" s="23" t="s">
         <v>7</v>
@@ -5585,7 +5592,7 @@
         <v>55</v>
       </c>
       <c r="C55" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D55" s="27" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
updated figures and statistics table
</commit_message>
<xml_diff>
--- a/FishLandings/household groups/statistics summary.xlsx
+++ b/FishLandings/household groups/statistics summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Kenya_SamakiSalama\FishLandings\household groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CAE58B-10C0-4E57-A868-B076702D68E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1CFC4A-D8FC-4864-930B-402529B38E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31125" yWindow="3390" windowWidth="21600" windowHeight="11235" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="118">
   <si>
     <t>Effect</t>
   </si>
@@ -448,7 +448,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -612,11 +612,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -728,17 +752,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1021,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E06F813-7338-485B-A007-E93757D85C7B}">
-  <dimension ref="B3:F63"/>
+  <dimension ref="B3:M66"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,10 +1083,16 @@
     <col min="4" max="4" width="25.44140625" style="62" customWidth="1"/>
     <col min="5" max="5" width="25.44140625" style="16" customWidth="1"/>
     <col min="6" max="6" width="15" style="16" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="16"/>
+    <col min="7" max="8" width="8.88671875" style="16"/>
+    <col min="9" max="9" width="29.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="16" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" style="62" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="15" style="16" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="44" t="s">
         <v>5</v>
       </c>
@@ -1054,8 +1108,23 @@
       <c r="F3" s="37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I3" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
@@ -1071,8 +1140,23 @@
       <c r="F4" s="4">
         <v>0.10095899999999999</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I4" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="31">
+        <v>0.74869600000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="45"/>
       <c r="C5" s="54" t="s">
         <v>52</v>
@@ -1086,8 +1170,21 @@
       <c r="F5" s="4">
         <v>0.10519000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I5" s="45"/>
+      <c r="J5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="34">
+        <v>5.862E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="46"/>
       <c r="C6" s="55" t="s">
         <v>55</v>
@@ -1101,8 +1198,21 @@
       <c r="F6" s="14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I6" s="46"/>
+      <c r="J6" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="35">
+        <v>4.052E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1118,8 +1228,23 @@
       <c r="F7" s="31">
         <v>0.16929900000000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="31">
+        <v>0.36364000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="45"/>
       <c r="C8" s="54" t="s">
         <v>52</v>
@@ -1133,8 +1258,21 @@
       <c r="F8" s="31">
         <v>0.84406199999999998</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I8" s="45"/>
+      <c r="J8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="31">
+        <v>0.14141100000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="46"/>
       <c r="C9" s="55" t="s">
         <v>55</v>
@@ -1148,8 +1286,21 @@
       <c r="F9" s="35">
         <v>9.6620000000000004E-3</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I9" s="46"/>
+      <c r="J9" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="35">
+        <v>1.22E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
@@ -1165,8 +1316,23 @@
       <c r="F10" s="31">
         <v>8.9454000000000006E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="31">
+        <v>0.10566200000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="45"/>
       <c r="C11" s="54" t="s">
         <v>52</v>
@@ -1180,8 +1346,21 @@
       <c r="F11" s="31">
         <v>0.98400900000000002</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I11" s="45"/>
+      <c r="J11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="31">
+        <v>0.96443699999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="46"/>
       <c r="C12" s="55" t="s">
         <v>55</v>
@@ -1195,8 +1374,21 @@
       <c r="F12" s="35">
         <v>1.4345E-2</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I12" s="46"/>
+      <c r="J12" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="35">
+        <v>1.3528E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>24</v>
       </c>
@@ -1212,8 +1404,23 @@
       <c r="F13" s="31">
         <v>0.11010300000000001</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="31">
+        <v>0.40166299999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="45"/>
       <c r="C14" s="54" t="s">
         <v>52</v>
@@ -1227,8 +1434,21 @@
       <c r="F14" s="31">
         <v>0.45139099999999999</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I14" s="45"/>
+      <c r="J14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="31">
+        <v>0.51743799999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="46"/>
       <c r="C15" s="55" t="s">
         <v>55</v>
@@ -1242,8 +1462,21 @@
       <c r="F15" s="35">
         <v>1.9000000000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I15" s="45"/>
+      <c r="J15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="31">
+        <v>0.989846</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>25</v>
       </c>
@@ -1259,8 +1492,23 @@
       <c r="F16" s="31">
         <v>7.8071000000000002E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I16" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="L16" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="76">
+        <v>0.26283600000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="45"/>
       <c r="C17" s="54" t="s">
         <v>52</v>
@@ -1274,8 +1522,21 @@
       <c r="F17" s="31">
         <v>0.44097399999999998</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I17" s="45"/>
+      <c r="J17" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="31">
+        <v>0.67078199999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="46"/>
       <c r="C18" s="55" t="s">
         <v>55</v>
@@ -1289,8 +1550,21 @@
       <c r="F18" s="35">
         <v>8.0000000000000007E-5</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I18" s="46"/>
+      <c r="J18" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="32">
+        <v>0.70625599999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1306,8 +1580,13 @@
       <c r="F19" s="31">
         <v>0.26812000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I19" s="68"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="71"/>
+    </row>
+    <row r="20" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="45"/>
       <c r="C20" s="54" t="s">
         <v>52</v>
@@ -1321,8 +1600,13 @@
       <c r="F20" s="31">
         <v>0.48186200000000001</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I20" s="72"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="71"/>
+    </row>
+    <row r="21" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="46"/>
       <c r="C21" s="55" t="s">
         <v>55</v>
@@ -1336,8 +1620,13 @@
       <c r="F21" s="35">
         <v>2.0330000000000001E-3</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I21" s="72"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="82"/>
+    </row>
+    <row r="22" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>27</v>
       </c>
@@ -1353,8 +1642,13 @@
       <c r="F22" s="31">
         <v>0.14516299999999999</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I22" s="68"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="71"/>
+    </row>
+    <row r="23" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="45"/>
       <c r="C23" s="54" t="s">
         <v>52</v>
@@ -1368,8 +1662,13 @@
       <c r="F23" s="31">
         <v>0.97426599999999997</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I23" s="72"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="71"/>
+    </row>
+    <row r="24" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="46"/>
       <c r="C24" s="55" t="s">
         <v>55</v>
@@ -1383,8 +1682,13 @@
       <c r="F24" s="35">
         <v>2.648E-2</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I24" s="72"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="82"/>
+    </row>
+    <row r="25" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="48" t="s">
         <v>30</v>
       </c>
@@ -1400,8 +1704,13 @@
       <c r="F25" s="42">
         <v>5.6696000000000003E-2</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I25" s="73"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
+    </row>
+    <row r="26" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="45"/>
       <c r="C26" s="54" t="s">
         <v>52</v>
@@ -1415,8 +1724,13 @@
       <c r="F26" s="31">
         <v>0.793767</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I26" s="72"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="70"/>
+      <c r="M26" s="71"/>
+    </row>
+    <row r="27" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="46"/>
       <c r="C27" s="55" t="s">
         <v>55</v>
@@ -1430,8 +1744,13 @@
       <c r="F27" s="32">
         <v>0.119883</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I27" s="72"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="70"/>
+      <c r="M27" s="71"/>
+    </row>
+    <row r="28" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>31</v>
       </c>
@@ -1447,8 +1766,13 @@
       <c r="F28" s="42">
         <v>6.5806000000000003E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I28" s="68"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="74"/>
+    </row>
+    <row r="29" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="45"/>
       <c r="C29" s="54" t="s">
         <v>52</v>
@@ -1462,8 +1786,13 @@
       <c r="F29" s="31">
         <v>0.48275299999999999</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I29" s="72"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="71"/>
+    </row>
+    <row r="30" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="46"/>
       <c r="C30" s="55" t="s">
         <v>55</v>
@@ -1477,8 +1806,13 @@
       <c r="F30" s="35">
         <v>8.1000000000000004E-5</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I30" s="72"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="82"/>
+    </row>
+    <row r="31" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>32</v>
       </c>
@@ -1494,8 +1828,13 @@
       <c r="F31" s="31">
         <v>0.74869600000000003</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
+    </row>
+    <row r="32" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="45"/>
       <c r="C32" s="54" t="s">
         <v>52</v>
@@ -1509,8 +1848,13 @@
       <c r="F32" s="34">
         <v>5.862E-3</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="72"/>
+    </row>
+    <row r="33" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="46"/>
       <c r="C33" s="55" t="s">
         <v>55</v>
@@ -1524,8 +1868,13 @@
       <c r="F33" s="35">
         <v>4.052E-3</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="72"/>
+    </row>
+    <row r="34" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>34</v>
       </c>
@@ -1541,8 +1890,13 @@
       <c r="F34" s="31">
         <v>0.36364000000000002</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I34" s="72"/>
+      <c r="J34" s="72"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="72"/>
+    </row>
+    <row r="35" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="45"/>
       <c r="C35" s="54" t="s">
         <v>52</v>
@@ -1556,8 +1910,13 @@
       <c r="F35" s="31">
         <v>0.14141100000000001</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="75"/>
+      <c r="L35" s="72"/>
+      <c r="M35" s="72"/>
+    </row>
+    <row r="36" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="46"/>
       <c r="C36" s="55" t="s">
         <v>55</v>
@@ -1571,8 +1930,13 @@
       <c r="F36" s="35">
         <v>1.22E-4</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="72"/>
+    </row>
+    <row r="37" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>36</v>
       </c>
@@ -1588,8 +1952,13 @@
       <c r="F37" s="31">
         <v>0.10566200000000001</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+    </row>
+    <row r="38" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="45"/>
       <c r="C38" s="54" t="s">
         <v>52</v>
@@ -1603,8 +1972,13 @@
       <c r="F38" s="31">
         <v>0.96443699999999999</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I38" s="72"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="72"/>
+    </row>
+    <row r="39" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="46"/>
       <c r="C39" s="55" t="s">
         <v>55</v>
@@ -1618,8 +1992,13 @@
       <c r="F39" s="35">
         <v>1.3528E-2</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="72"/>
+      <c r="M39" s="72"/>
+    </row>
+    <row r="40" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
         <v>37</v>
       </c>
@@ -1635,8 +2014,13 @@
       <c r="F40" s="31">
         <v>0.40166299999999999</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="72"/>
+      <c r="M40" s="72"/>
+    </row>
+    <row r="41" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="45"/>
       <c r="C41" s="54" t="s">
         <v>52</v>
@@ -1650,8 +2034,13 @@
       <c r="F41" s="31">
         <v>0.51743799999999995</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="72"/>
+      <c r="M41" s="72"/>
+    </row>
+    <row r="42" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="46"/>
       <c r="C42" s="55" t="s">
         <v>55</v>
@@ -1665,8 +2054,13 @@
       <c r="F42" s="32">
         <v>0.989846</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+    </row>
+    <row r="43" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>38</v>
       </c>
@@ -1682,8 +2076,13 @@
       <c r="F43" s="31">
         <v>0.26283600000000001</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="72"/>
+    </row>
+    <row r="44" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B44" s="45"/>
       <c r="C44" s="54" t="s">
         <v>52</v>
@@ -1697,8 +2096,13 @@
       <c r="F44" s="31">
         <v>0.67078199999999999</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I44" s="72"/>
+      <c r="J44" s="72"/>
+      <c r="K44" s="75"/>
+      <c r="L44" s="72"/>
+      <c r="M44" s="72"/>
+    </row>
+    <row r="45" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="46"/>
       <c r="C45" s="55" t="s">
         <v>55</v>
@@ -1712,8 +2116,13 @@
       <c r="F45" s="32">
         <v>0.70625599999999999</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I45" s="72"/>
+      <c r="J45" s="72"/>
+      <c r="K45" s="75"/>
+      <c r="L45" s="72"/>
+      <c r="M45" s="72"/>
+    </row>
+    <row r="46" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
         <v>42</v>
       </c>
@@ -1723,14 +2132,19 @@
       <c r="D46" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="53" t="s">
+      <c r="E46" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="34">
+      <c r="F46" s="67">
         <v>8.1814999999999999E-2</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I46" s="68"/>
+      <c r="J46" s="69"/>
+      <c r="K46" s="69"/>
+      <c r="L46" s="73"/>
+      <c r="M46" s="74"/>
+    </row>
+    <row r="47" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B47" s="45"/>
       <c r="C47" s="54" t="s">
         <v>52</v>
@@ -1744,8 +2158,13 @@
       <c r="F47" s="31">
         <v>0.76895000000000002</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I47" s="72"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="69"/>
+      <c r="L47" s="70"/>
+      <c r="M47" s="71"/>
+    </row>
+    <row r="48" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="46"/>
       <c r="C48" s="55" t="s">
         <v>55</v>
@@ -1759,8 +2178,13 @@
       <c r="F48" s="35">
         <v>1.32E-3</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I48" s="72"/>
+      <c r="J48" s="69"/>
+      <c r="K48" s="69"/>
+      <c r="L48" s="68"/>
+      <c r="M48" s="82"/>
+    </row>
+    <row r="49" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B49" s="7" t="s">
         <v>43</v>
       </c>
@@ -1776,8 +2200,13 @@
       <c r="F49" s="31">
         <v>0.97677599999999998</v>
       </c>
-    </row>
-    <row r="50" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I49" s="68"/>
+      <c r="J49" s="69"/>
+      <c r="K49" s="69"/>
+      <c r="L49" s="70"/>
+      <c r="M49" s="71"/>
+    </row>
+    <row r="50" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B50" s="45"/>
       <c r="C50" s="54" t="s">
         <v>52</v>
@@ -1791,8 +2220,13 @@
       <c r="F50" s="34">
         <v>7.3119999999999999E-3</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I50" s="72"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="69"/>
+      <c r="L50" s="68"/>
+      <c r="M50" s="82"/>
+    </row>
+    <row r="51" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B51" s="46"/>
       <c r="C51" s="55" t="s">
         <v>55</v>
@@ -1803,11 +2237,16 @@
       <c r="E51" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F51" s="67" t="s">
+      <c r="F51" s="63" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I51" s="72"/>
+      <c r="J51" s="69"/>
+      <c r="K51" s="69"/>
+      <c r="L51" s="68"/>
+      <c r="M51" s="83"/>
+    </row>
+    <row r="52" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="7" t="s">
         <v>44</v>
       </c>
@@ -1823,8 +2262,13 @@
       <c r="F52" s="34">
         <v>4.7930000000000004E-3</v>
       </c>
-    </row>
-    <row r="53" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I52" s="68"/>
+      <c r="J52" s="69"/>
+      <c r="K52" s="69"/>
+      <c r="L52" s="68"/>
+      <c r="M52" s="82"/>
+    </row>
+    <row r="53" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B53" s="45"/>
       <c r="C53" s="54" t="s">
         <v>52</v>
@@ -1838,8 +2282,13 @@
       <c r="F53" s="31">
         <v>0.99937500000000001</v>
       </c>
-    </row>
-    <row r="54" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I53" s="72"/>
+      <c r="J53" s="69"/>
+      <c r="K53" s="69"/>
+      <c r="L53" s="70"/>
+      <c r="M53" s="71"/>
+    </row>
+    <row r="54" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B54" s="46"/>
       <c r="C54" s="55" t="s">
         <v>55</v>
@@ -1853,8 +2302,13 @@
       <c r="F54" s="35">
         <v>4.35E-4</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I54" s="72"/>
+      <c r="J54" s="69"/>
+      <c r="K54" s="69"/>
+      <c r="L54" s="68"/>
+      <c r="M54" s="82"/>
+    </row>
+    <row r="55" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
         <v>46</v>
       </c>
@@ -1870,8 +2324,13 @@
       <c r="F55" s="31">
         <v>0.719831</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I55" s="70"/>
+      <c r="J55" s="69"/>
+      <c r="K55" s="69"/>
+      <c r="L55" s="70"/>
+      <c r="M55" s="71"/>
+    </row>
+    <row r="56" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B56" s="45"/>
       <c r="C56" s="54" t="s">
         <v>52</v>
@@ -1885,8 +2344,13 @@
       <c r="F56" s="31">
         <v>0.20863300000000001</v>
       </c>
-    </row>
-    <row r="57" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I56" s="72"/>
+      <c r="J56" s="69"/>
+      <c r="K56" s="69"/>
+      <c r="L56" s="70"/>
+      <c r="M56" s="71"/>
+    </row>
+    <row r="57" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B57" s="46"/>
       <c r="C57" s="55" t="s">
         <v>55</v>
@@ -1900,8 +2364,13 @@
       <c r="F57" s="32">
         <v>0.39966299999999999</v>
       </c>
-    </row>
-    <row r="58" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I57" s="72"/>
+      <c r="J57" s="69"/>
+      <c r="K57" s="69"/>
+      <c r="L57" s="70"/>
+      <c r="M57" s="71"/>
+    </row>
+    <row r="58" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B58" s="7" t="s">
         <v>48</v>
       </c>
@@ -1917,8 +2386,13 @@
       <c r="F58" s="31">
         <v>0.93880200000000003</v>
       </c>
-    </row>
-    <row r="59" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I58" s="68"/>
+      <c r="J58" s="69"/>
+      <c r="K58" s="69"/>
+      <c r="L58" s="70"/>
+      <c r="M58" s="71"/>
+    </row>
+    <row r="59" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B59" s="45"/>
       <c r="C59" s="54" t="s">
         <v>52</v>
@@ -1932,8 +2406,13 @@
       <c r="F59" s="34">
         <v>1.7291000000000001E-2</v>
       </c>
-    </row>
-    <row r="60" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I59" s="72"/>
+      <c r="J59" s="69"/>
+      <c r="K59" s="69"/>
+      <c r="L59" s="68"/>
+      <c r="M59" s="82"/>
+    </row>
+    <row r="60" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B60" s="46"/>
       <c r="C60" s="55" t="s">
         <v>55</v>
@@ -1947,8 +2426,13 @@
       <c r="F60" s="35">
         <v>1.9799999999999999E-4</v>
       </c>
-    </row>
-    <row r="61" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I60" s="72"/>
+      <c r="J60" s="69"/>
+      <c r="K60" s="69"/>
+      <c r="L60" s="68"/>
+      <c r="M60" s="82"/>
+    </row>
+    <row r="61" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B61" s="7" t="s">
         <v>50</v>
       </c>
@@ -1964,8 +2448,13 @@
       <c r="F61" s="34">
         <v>3.3382000000000002E-2</v>
       </c>
-    </row>
-    <row r="62" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I61" s="68"/>
+      <c r="J61" s="69"/>
+      <c r="K61" s="69"/>
+      <c r="L61" s="68"/>
+      <c r="M61" s="82"/>
+    </row>
+    <row r="62" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B62" s="45"/>
       <c r="C62" s="54" t="s">
         <v>52</v>
@@ -1979,8 +2468,13 @@
       <c r="F62" s="31">
         <v>0.77748200000000001</v>
       </c>
-    </row>
-    <row r="63" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I62" s="72"/>
+      <c r="J62" s="69"/>
+      <c r="K62" s="69"/>
+      <c r="L62" s="70"/>
+      <c r="M62" s="71"/>
+    </row>
+    <row r="63" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B63" s="46"/>
       <c r="C63" s="55" t="s">
         <v>55</v>
@@ -1994,6 +2488,32 @@
       <c r="F63" s="35">
         <v>2.6600000000000001E-4</v>
       </c>
+      <c r="I63" s="72"/>
+      <c r="J63" s="69"/>
+      <c r="K63" s="69"/>
+      <c r="L63" s="68"/>
+      <c r="M63" s="82"/>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I64" s="72"/>
+      <c r="J64" s="72"/>
+      <c r="K64" s="75"/>
+      <c r="L64" s="72"/>
+      <c r="M64" s="72"/>
+    </row>
+    <row r="65" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I65" s="72"/>
+      <c r="J65" s="72"/>
+      <c r="K65" s="75"/>
+      <c r="L65" s="72"/>
+      <c r="M65" s="72"/>
+    </row>
+    <row r="66" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I66" s="72"/>
+      <c r="J66" s="72"/>
+      <c r="K66" s="75"/>
+      <c r="L66" s="72"/>
+      <c r="M66" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2005,7 +2525,7 @@
   <dimension ref="B1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2021,15 +2541,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="3" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
@@ -2400,7 +2920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C378BB95-8E32-43A5-9776-0E3CD4F07137}">
   <dimension ref="B1:H64"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -2417,15 +2937,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="3" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="17" t="s">
@@ -3620,15 +4140,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="3" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="17" t="s">
@@ -4586,7 +5106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FFC064-2F91-4093-9CA2-53F2C36B19E0}">
   <dimension ref="B1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -4604,15 +5124,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="3" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="17" t="s">
@@ -4809,13 +5329,13 @@
       <c r="D13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="22">
         <v>0.80072299999999996</v>
       </c>
-      <c r="F13" s="64">
+      <c r="F13" s="22">
         <v>1</v>
       </c>
-      <c r="G13" s="64">
+      <c r="G13" s="22">
         <v>2.3380879999999999</v>
       </c>
       <c r="H13" s="31">
@@ -4830,16 +5350,16 @@
       <c r="D14" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="68">
+      <c r="E14" s="30">
         <v>10.704165</v>
       </c>
-      <c r="F14" s="68">
+      <c r="F14" s="30">
         <v>2</v>
       </c>
-      <c r="G14" s="68">
+      <c r="G14" s="30">
         <v>15.627917999999999</v>
       </c>
-      <c r="H14" s="69" t="s">
+      <c r="H14" s="64" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4849,13 +5369,13 @@
       <c r="D15" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="22">
         <v>16.096057999999999</v>
       </c>
-      <c r="F15" s="64">
+      <c r="F15" s="22">
         <v>47</v>
       </c>
-      <c r="G15" s="64"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4887,13 +5407,13 @@
       <c r="D17" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="25">
         <v>6.7158999999999996E-2</v>
       </c>
-      <c r="F17" s="65">
+      <c r="F17" s="25">
         <v>-0.71989300000000001</v>
       </c>
-      <c r="G17" s="65">
+      <c r="G17" s="25">
         <v>0.85421000000000002</v>
       </c>
       <c r="H17" s="31">
@@ -4910,13 +5430,13 @@
       <c r="D18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="43">
         <v>0.99118700000000004</v>
       </c>
-      <c r="F18" s="66">
+      <c r="F18" s="43">
         <v>0.235788</v>
       </c>
-      <c r="G18" s="66">
+      <c r="G18" s="43">
         <v>1.7465850000000001</v>
       </c>
       <c r="H18" s="34">
@@ -4942,7 +5462,7 @@
       <c r="G19" s="28">
         <v>1.3566450000000001</v>
       </c>
-      <c r="H19" s="67" t="s">
+      <c r="H19" s="63" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>